<commit_message>
letní semestr 2024 info kombi
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>Den</t>
   </si>
@@ -43,22 +43,22 @@
     <t>Kapacita</t>
   </si>
   <si>
-    <t>So 07.10.2023</t>
+    <t>So 17.02.2024</t>
   </si>
   <si>
     <t>08:45</t>
   </si>
   <si>
-    <t>15:45</t>
-  </si>
-  <si>
-    <t>EIED8E Business Intelligence - INFON3 kombi.</t>
+    <t>16:45</t>
+  </si>
+  <si>
+    <t>EIE87E Systémová integrace - INFON4 komb.</t>
   </si>
   <si>
     <t>Přednáška</t>
   </si>
   <si>
-    <t>PEF DI</t>
+    <t>AII</t>
   </si>
   <si>
     <t>Tyrychtr Jan</t>
@@ -67,91 +67,91 @@
     <t>2n-infonp</t>
   </si>
   <si>
-    <t>Pá 03.11.2023</t>
-  </si>
-  <si>
-    <t>14:00</t>
+    <t>Ne 18.02.2024</t>
+  </si>
+  <si>
+    <t>EIEB7E Gramatiky a jazyky - INFON4 komb.</t>
+  </si>
+  <si>
+    <t>PEF C11</t>
+  </si>
+  <si>
+    <t>Merunka Vojtěch</t>
+  </si>
+  <si>
+    <t>Pá 08.03.2024</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
+    <t>20:15</t>
+  </si>
+  <si>
+    <t>ETEW8E Zpracování velkých dat - INFON4v Kombi.</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Masner Jan</t>
+  </si>
+  <si>
+    <t>So 09.03.2024</t>
+  </si>
+  <si>
+    <t>ETE90E Internetové technologie - server side - INFON4k komb.</t>
+  </si>
+  <si>
+    <t>Lohr Václav</t>
+  </si>
+  <si>
+    <t>Ne 10.03.2024</t>
+  </si>
+  <si>
+    <t>EJE98E Právní aspekty IT INFON4 DS</t>
+  </si>
+  <si>
+    <t>Reichert Michal</t>
+  </si>
+  <si>
+    <t>Pá 05.04.2024</t>
+  </si>
+  <si>
+    <t>13:00</t>
   </si>
   <si>
     <t>21:00</t>
   </si>
   <si>
-    <t>EAEB2E Logistické systémy - INFON3v komb.</t>
-  </si>
-  <si>
-    <t>Šubrt Tomáš</t>
-  </si>
-  <si>
-    <t>2n-infonp1</t>
-  </si>
-  <si>
-    <t>ESEA1E Statistická analýza dat - INFON1 komb.</t>
+    <t>Cvičení</t>
+  </si>
+  <si>
+    <t>So 06.04.2024</t>
+  </si>
+  <si>
+    <t>ETE90E Internetové technologie - server side - INFON4k komb. (1)</t>
+  </si>
+  <si>
+    <t>Ne 07.04.2024</t>
   </si>
   <si>
     <t>PEF EII</t>
   </si>
   <si>
-    <t>Špička Jindřich</t>
-  </si>
-  <si>
-    <t>1n-infonp</t>
-  </si>
-  <si>
-    <t>So 04.11.2023</t>
-  </si>
-  <si>
-    <t>EIED9E Formální techniky datového modelování - INFON3 kombi.</t>
-  </si>
-  <si>
-    <t>Merunka Vojtěch</t>
-  </si>
-  <si>
-    <t>Ne 05.11.2023</t>
-  </si>
-  <si>
-    <t>ESED5E Data Mining - INFON3 - kombi</t>
-  </si>
-  <si>
-    <t>Pacáková Zuzana</t>
-  </si>
-  <si>
-    <t>Pá 10.11.2023</t>
-  </si>
-  <si>
-    <t>14:45</t>
-  </si>
-  <si>
-    <t>21:45</t>
-  </si>
-  <si>
-    <t>Cvičení</t>
-  </si>
-  <si>
-    <t>PEF EIII</t>
-  </si>
-  <si>
-    <t>So 11.11.2023</t>
-  </si>
-  <si>
-    <t>Pá 01.12.2023</t>
-  </si>
-  <si>
-    <t>ETE89E Internetové technologie - client side - INFON3k komb.</t>
-  </si>
-  <si>
-    <t>PEF EV</t>
-  </si>
-  <si>
-    <t>Lohr Václav</t>
-  </si>
-  <si>
-    <t>So 02.12.2023</t>
-  </si>
-  <si>
-    <t>Ne 03.12.2023</t>
-  </si>
-  <si>
-    <t>Po 08.01.2024</t>
+    <t>Pá 26.04.2024</t>
+  </si>
+  <si>
+    <t>13:05</t>
+  </si>
+  <si>
+    <t>21:05</t>
+  </si>
+  <si>
+    <t>AIII</t>
+  </si>
+  <si>
+    <t>Ne 28.04.2024</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,11 +538,11 @@
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -607,58 +607,54 @@
         <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="2">
-        <v>60</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="2">
-        <v>60</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
@@ -677,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>29</v>
@@ -704,7 +700,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>32</v>
@@ -725,16 +721,16 @@
         <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>16</v>
@@ -743,7 +739,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -752,74 +748,70 @@
         <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="2">
-        <v>60</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G9" s="5" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="2">
-        <v>60</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>16</v>
@@ -828,7 +820,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -837,79 +829,21 @@
         <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="2">
-        <v>60</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>